<commit_message>
Visu Home + admin page
</commit_message>
<xml_diff>
--- a/backend/courses.xlsx
+++ b/backend/courses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Utilisateurs" sheetId="1" r:id="rId1"/>
+    <sheet name="Courses" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,39 +412,230 @@
       <c r="C1" t="str">
         <v>quantity</v>
       </c>
-      <c r="D1" t="str">
-        <v>gear</v>
-      </c>
-      <c r="E1" t="str">
-        <v>presenceDays</v>
-      </c>
-      <c r="F1" t="str">
-        <v>transactions</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>1745434465793</v>
+        <v>1745483727576</v>
       </c>
       <c r="B2" t="str">
-        <v>Bière</v>
+        <v>Gruyère (kg)</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1745483739301</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Bolo (pot)</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1745483754454</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Sauce tomate (pot)</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1745483763510</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Pesto verde (pot)</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1745483768824</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Pesto rouge (pot)</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1745483782830</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Beurre (plaquette)</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1745483808182</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Jambon (tranche)</v>
+      </c>
+      <c r="C8">
         <v>20</v>
       </c>
-      <c r="D2" t="str">
-        <v>[]</v>
-      </c>
-      <c r="E2" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F2" t="str">
-        <v>[]</v>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1745483815286</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Fromage (tranche)</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1745483829826</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Chips (paquet)</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1745483841437</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Nutella (pot)</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>1745483857388</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Bière (L)</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>1745483866138</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Vodka (L)</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>1745483888070</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Smirnoff (Bouteille)</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>1745483896109</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Bulles (Bouteille)</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>1745483904748</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Ricard (Bouteille)</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>1745483912320</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Grenadine (Bouteille)</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>1745483920571</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Jaeger (Bouteille)</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>1745483927641</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Limonade (Bouteille)</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>1745483935346</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Taurine (Bouteille)</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>1745486439425</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Multifruit (Bouteille)</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>